<commit_message>
Analysis of 10 TPAs
</commit_message>
<xml_diff>
--- a/Extraction_details.xlsx
+++ b/Extraction_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\INTERNSHIP\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016C9735-713E-4E39-88BB-182F049EC002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BFF3FD-C7B3-46A6-82C4-08B5E5F860D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,7 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -608,16 +608,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -629,9 +626,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -916,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -976,193 +975,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="8" t="s">
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="4" t="s">
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="4" t="s">
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="4"/>
-      <c r="AT1" s="4"/>
-      <c r="AU1" s="4" t="s">
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
+      <c r="AU1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AV1" s="4"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="4"/>
-      <c r="AY1" s="4"/>
+      <c r="AV1" s="6"/>
+      <c r="AW1" s="6"/>
+      <c r="AX1" s="6"/>
+      <c r="AY1" s="6"/>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4" t="s">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4" t="s">
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="5" t="s">
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="5" t="s">
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AO2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AP2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="5" t="s">
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AT2" s="5" t="s">
+      <c r="AT2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AU2" s="8" t="s">
+      <c r="AU2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="5" t="s">
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AY2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1172,8 +1171,8 @@
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1183,8 +1182,8 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1194,8 +1193,8 @@
       <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
       <c r="Q3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1205,8 +1204,8 @@
       <c r="S3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
       <c r="V3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1216,8 +1215,8 @@
       <c r="X3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
       <c r="AA3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1227,8 +1226,8 @@
       <c r="AC3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
       <c r="AF3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1238,8 +1237,8 @@
       <c r="AH3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
       <c r="AK3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1249,8 +1248,8 @@
       <c r="AM3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
       <c r="AP3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1260,8 +1259,8 @@
       <c r="AR3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="7"/>
-      <c r="AT3" s="7"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
       <c r="AU3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1271,8 +1270,8 @@
       <c r="AW3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AX3" s="7"/>
-      <c r="AY3" s="7"/>
+      <c r="AX3" s="5"/>
+      <c r="AY3" s="5"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -2158,13 +2157,13 @@
       <c r="AJ9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK9" s="11" t="s">
+      <c r="AK9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AL9" s="11" t="s">
+      <c r="AL9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM9" s="11" t="s">
+      <c r="AM9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AN9" s="1" t="s">
@@ -2313,10 +2312,10 @@
       <c r="AJ10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK10" s="12" t="s">
+      <c r="AK10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AL10" s="12" t="s">
+      <c r="AL10" s="4" t="s">
         <v>105</v>
       </c>
       <c r="AM10" s="1" t="s">
@@ -2468,8 +2467,8 @@
       <c r="AJ11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK11" s="7"/>
-      <c r="AL11" s="7"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
       <c r="AM11" s="1" t="s">
         <v>108</v>
       </c>
@@ -3132,24 +3131,15 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Y3"/>
     <mergeCell ref="AA1:AE1"/>
     <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="AD2:AD3"/>
@@ -3166,15 +3156,24 @@
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new TPA
</commit_message>
<xml_diff>
--- a/Extraction_details.xlsx
+++ b/Extraction_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\INTERNSHIP\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BFF3FD-C7B3-46A6-82C4-08B5E5F860D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E45F4-8203-41CB-92C5-A1BDC17D3EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="157">
   <si>
     <t>ICICI</t>
   </si>
@@ -461,6 +461,42 @@
   </si>
   <si>
     <t>Next line after "AL Approved Date"</t>
+  </si>
+  <si>
+    <t>MEDIASSIST</t>
+  </si>
+  <si>
+    <t>Cashless Claim Reference Number</t>
+  </si>
+  <si>
+    <t>Medi Assist ID</t>
+  </si>
+  <si>
+    <t>Next line after "We regret to inform you"</t>
+  </si>
+  <si>
+    <t>Next line after " We require the following additional information"</t>
+  </si>
+  <si>
+    <t>Date :</t>
+  </si>
+  <si>
+    <t>In brackets after "Cashless Authorization Letter"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Authorized amount </t>
+  </si>
+  <si>
+    <t>Policy/Plan Period</t>
+  </si>
+  <si>
+    <t>Estimated/Actual Date of Discharge</t>
+  </si>
+  <si>
+    <t>Estimated Date of Discharge</t>
+  </si>
+  <si>
+    <t>Expected/Actual Date Of Admission</t>
   </si>
 </sst>
 </file>
@@ -608,13 +644,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -627,10 +666,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -913,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:BD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="BB20" sqref="BB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,196 +1008,219 @@
     <col min="49" max="49" width="37.6328125" customWidth="1"/>
     <col min="50" max="50" width="39.36328125" customWidth="1"/>
     <col min="51" max="51" width="39.6328125" customWidth="1"/>
+    <col min="52" max="52" width="41.90625" customWidth="1"/>
+    <col min="53" max="53" width="41.54296875" customWidth="1"/>
+    <col min="54" max="54" width="41.6328125" customWidth="1"/>
+    <col min="55" max="55" width="35.90625" customWidth="1"/>
+    <col min="56" max="56" width="55.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="7" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="6" t="s">
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6" t="s">
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6" t="s">
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
+      <c r="AV1" s="4"/>
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="A2" s="6"/>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6" t="s">
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6" t="s">
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6" t="s">
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AF2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="10" t="s">
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="10" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AO2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="10" t="s">
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AT2" s="10" t="s">
+      <c r="AT2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AU2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="10" t="s">
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="10" t="s">
+      <c r="AY2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AZ2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1171,8 +1230,8 @@
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1182,8 +1241,8 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
       <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1193,8 +1252,8 @@
       <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1204,8 +1263,8 @@
       <c r="S3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
       <c r="V3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1215,8 +1274,8 @@
       <c r="X3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
       <c r="AA3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1226,8 +1285,8 @@
       <c r="AC3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
       <c r="AF3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1237,8 +1296,8 @@
       <c r="AH3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
       <c r="AK3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1248,8 +1307,8 @@
       <c r="AM3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="5"/>
-      <c r="AO3" s="5"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
       <c r="AP3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1259,8 +1318,8 @@
       <c r="AR3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="5"/>
-      <c r="AT3" s="5"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
       <c r="AU3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1270,10 +1329,21 @@
       <c r="AW3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AX3" s="5"/>
-      <c r="AY3" s="5"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1427,8 +1497,23 @@
       <c r="AY4" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AZ4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1582,8 +1667,23 @@
       <c r="AY5" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="AZ5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BC5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="BD5" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1737,8 +1837,23 @@
       <c r="AY6" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="AZ6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BC6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD6" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1892,8 +2007,23 @@
       <c r="AY7" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AZ7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD7" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2047,8 +2177,23 @@
       <c r="AY8" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="AZ8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BB8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD8" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2202,8 +2347,23 @@
       <c r="AY9" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AZ9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BC9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD9" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -2312,10 +2472,10 @@
       <c r="AJ10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AK10" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="AL10" s="4" t="s">
+      <c r="AL10" s="11" t="s">
         <v>105</v>
       </c>
       <c r="AM10" s="1" t="s">
@@ -2357,8 +2517,23 @@
       <c r="AY10" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="AZ10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BC10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD10" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2467,8 +2642,8 @@
       <c r="AJ11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="5"/>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
       <c r="AM11" s="1" t="s">
         <v>108</v>
       </c>
@@ -2508,8 +2683,23 @@
       <c r="AY11" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AZ11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BA11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BC11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD11" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2663,8 +2853,23 @@
       <c r="AY12" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AZ12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BC12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD12" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
@@ -2818,8 +3023,23 @@
       <c r="AY13" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="AZ13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BD13" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -2968,13 +3188,28 @@
         <v>131</v>
       </c>
       <c r="AX14" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="AY14" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="AZ14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD14" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -3128,18 +3363,46 @@
       <c r="AY15" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AZ15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BB15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD15" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:Y3"/>
+  <mergeCells count="47">
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="AZ2:BB2"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK1:AO1"/>
     <mergeCell ref="AA1:AE1"/>
     <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="AD2:AD3"/>
@@ -3156,24 +3419,15 @@
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Y3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Need to add one more TPA
</commit_message>
<xml_diff>
--- a/Extraction_details.xlsx
+++ b/Extraction_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\INTERNSHIP\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E45F4-8203-41CB-92C5-A1BDC17D3EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575AE6FB-CB6A-4E7B-AEE3-D5F1A3713D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="158">
   <si>
     <t>ICICI</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>Expected/Actual Date Of Admission</t>
+  </si>
+  <si>
+    <t>HDFC</t>
   </si>
 </sst>
 </file>
@@ -949,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD15"/>
+  <dimension ref="A1:BI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="BB20" sqref="BB20"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="83" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="BK20" sqref="BK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,12 +974,12 @@
     <col min="12" max="12" width="23.90625" customWidth="1"/>
     <col min="13" max="13" width="24.453125" customWidth="1"/>
     <col min="14" max="14" width="25.26953125" customWidth="1"/>
-    <col min="15" max="15" width="26.6328125" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" customWidth="1"/>
     <col min="16" max="16" width="45.81640625" customWidth="1"/>
     <col min="17" max="17" width="45.453125" customWidth="1"/>
     <col min="18" max="18" width="45.26953125" customWidth="1"/>
     <col min="19" max="19" width="45" customWidth="1"/>
-    <col min="20" max="20" width="28" customWidth="1"/>
+    <col min="20" max="20" width="24.453125" customWidth="1"/>
     <col min="21" max="21" width="27.81640625" customWidth="1"/>
     <col min="22" max="22" width="23.08984375" customWidth="1"/>
     <col min="23" max="23" width="22.90625" customWidth="1"/>
@@ -986,8 +989,8 @@
     <col min="27" max="27" width="46.26953125" customWidth="1"/>
     <col min="28" max="28" width="44.90625" customWidth="1"/>
     <col min="29" max="29" width="45.26953125" customWidth="1"/>
-    <col min="30" max="30" width="23.6328125" customWidth="1"/>
-    <col min="31" max="31" width="27.26953125" customWidth="1"/>
+    <col min="30" max="30" width="14.453125" customWidth="1"/>
+    <col min="31" max="31" width="23.6328125" customWidth="1"/>
     <col min="32" max="32" width="38.08984375" customWidth="1"/>
     <col min="33" max="33" width="28.90625" customWidth="1"/>
     <col min="34" max="34" width="29" customWidth="1"/>
@@ -1013,9 +1016,12 @@
     <col min="54" max="54" width="41.6328125" customWidth="1"/>
     <col min="55" max="55" width="35.90625" customWidth="1"/>
     <col min="56" max="56" width="55.453125" customWidth="1"/>
+    <col min="57" max="57" width="11.08984375" customWidth="1"/>
+    <col min="58" max="58" width="15.1796875" customWidth="1"/>
+    <col min="59" max="59" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1094,8 +1100,15 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
+      <c r="BE1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="BF1" s="9"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="10"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -1218,8 +1231,19 @@
       <c r="BD2" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="BE2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1342,8 +1366,19 @@
       </c>
       <c r="BC3" s="7"/>
       <c r="BD3" s="7"/>
+      <c r="BE3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1512,8 +1547,13 @@
       <c r="BD4" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1682,8 +1722,13 @@
       <c r="BD5" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1852,8 +1897,13 @@
       <c r="BD6" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2022,8 +2072,13 @@
       <c r="BD7" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2192,8 +2247,13 @@
       <c r="BD8" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2362,8 +2422,13 @@
       <c r="BD9" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -2532,8 +2597,13 @@
       <c r="BD10" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2698,8 +2768,13 @@
       <c r="BD11" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2868,8 +2943,13 @@
       <c r="BD12" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="1"/>
+      <c r="BG12" s="1"/>
+      <c r="BH12" s="1"/>
+      <c r="BI12" s="1"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
@@ -3038,8 +3118,13 @@
       <c r="BD13" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1"/>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -3208,8 +3293,13 @@
       <c r="BD14" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -3378,13 +3468,22 @@
       <c r="BD15" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="51">
+    <mergeCell ref="BE2:BG2"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="AZ2:BB2"/>
     <mergeCell ref="BC2:BC3"/>
     <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BE1:BI1"/>
     <mergeCell ref="AK10:AK11"/>
     <mergeCell ref="AL10:AL11"/>
     <mergeCell ref="AP1:AT1"/>

</xml_diff>

<commit_message>
Analysis of fields for 12 TPAs
</commit_message>
<xml_diff>
--- a/Extraction_details.xlsx
+++ b/Extraction_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\INTERNSHIP\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575AE6FB-CB6A-4E7B-AEE3-D5F1A3713D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21FB08E-4900-4355-A8C8-47EEA55F118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="170">
   <si>
     <t>ICICI</t>
   </si>
@@ -472,6 +472,9 @@
     <t>Medi Assist ID</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Next line after "We regret to inform you"</t>
   </si>
   <si>
@@ -500,6 +503,39 @@
   </si>
   <si>
     <t>HDFC</t>
+  </si>
+  <si>
+    <t>Next line after "To" (left side)</t>
+  </si>
+  <si>
+    <t>HDFC ERGO ID</t>
+  </si>
+  <si>
+    <t>After "Rejection of Cashless Claim facility for"</t>
+  </si>
+  <si>
+    <t>Next line after "due to following reasons:"</t>
+  </si>
+  <si>
+    <t>Next line after "provide the following information for processing the claim further."</t>
+  </si>
+  <si>
+    <t>After "Additional information required for cashless claim facility for"</t>
+  </si>
+  <si>
+    <t>Next line after "To" (left side of the table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy Number   </t>
+  </si>
+  <si>
+    <t>Expected Date of  Discharge</t>
+  </si>
+  <si>
+    <t>Patient's Member ID/TPA/Insurer Id of Patient</t>
   </si>
 </sst>
 </file>
@@ -638,7 +674,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -670,6 +706,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -952,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI15"/>
+  <dimension ref="A1:BK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="83" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="BK20" sqref="BK20"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="92" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="BF23" sqref="BF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1016,9 +1058,11 @@
     <col min="54" max="54" width="41.6328125" customWidth="1"/>
     <col min="55" max="55" width="35.90625" customWidth="1"/>
     <col min="56" max="56" width="55.453125" customWidth="1"/>
-    <col min="57" max="57" width="11.08984375" customWidth="1"/>
-    <col min="58" max="58" width="15.1796875" customWidth="1"/>
-    <col min="59" max="59" width="10.36328125" customWidth="1"/>
+    <col min="57" max="57" width="39.81640625" customWidth="1"/>
+    <col min="58" max="58" width="39.7265625" customWidth="1"/>
+    <col min="59" max="59" width="39.81640625" customWidth="1"/>
+    <col min="60" max="60" width="38.54296875" customWidth="1"/>
+    <col min="61" max="61" width="70.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.35">
@@ -1101,7 +1145,7 @@
       <c r="BC1" s="4"/>
       <c r="BD1" s="4"/>
       <c r="BE1" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BF1" s="9"/>
       <c r="BG1" s="9"/>
@@ -1369,7 +1413,7 @@
       <c r="BE3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="BF3" s="1" t="s">
+      <c r="BF3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="BG3" s="1" t="s">
@@ -1547,11 +1591,21 @@
       <c r="BD4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BE4" s="1"/>
-      <c r="BF4" s="1"/>
-      <c r="BG4" s="1"/>
-      <c r="BH4" s="1"/>
-      <c r="BI4" s="1"/>
+      <c r="BE4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BG4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BI4" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1708,13 +1762,13 @@
         <v>127</v>
       </c>
       <c r="AZ5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="BA5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="BC5" s="1" t="s">
         <v>146</v>
@@ -1722,11 +1776,21 @@
       <c r="BD5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BE5" s="1"/>
-      <c r="BF5" s="1"/>
-      <c r="BG5" s="1"/>
-      <c r="BH5" s="1"/>
-      <c r="BI5" s="1"/>
+      <c r="BE5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BG5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BH5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BI5" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1897,11 +1961,21 @@
       <c r="BD6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BE6" s="1"/>
-      <c r="BF6" s="1"/>
-      <c r="BG6" s="1"/>
-      <c r="BH6" s="1"/>
-      <c r="BI6" s="1"/>
+      <c r="BE6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="BG6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="BH6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="BI6" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -2072,11 +2146,21 @@
       <c r="BD7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="BE7" s="1"/>
-      <c r="BF7" s="1"/>
-      <c r="BG7" s="1"/>
-      <c r="BH7" s="1"/>
-      <c r="BI7" s="1"/>
+      <c r="BE7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="BH7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -2236,10 +2320,10 @@
         <v>26</v>
       </c>
       <c r="BA8" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="BB8" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="BC8" s="1" t="s">
         <v>37</v>
@@ -2247,11 +2331,21 @@
       <c r="BD8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BE8" s="1"/>
-      <c r="BF8" s="1"/>
-      <c r="BG8" s="1"/>
-      <c r="BH8" s="1"/>
-      <c r="BI8" s="1"/>
+      <c r="BE8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BH8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI8" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -2422,11 +2516,21 @@
       <c r="BD9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BE9" s="1"/>
-      <c r="BF9" s="1"/>
-      <c r="BG9" s="1"/>
-      <c r="BH9" s="1"/>
-      <c r="BI9" s="1"/>
+      <c r="BE9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI9" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -2589,7 +2693,7 @@
         <v>107</v>
       </c>
       <c r="BB10" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BC10" s="1" t="s">
         <v>37</v>
@@ -2597,11 +2701,21 @@
       <c r="BD10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BE10" s="1"/>
-      <c r="BF10" s="1"/>
-      <c r="BG10" s="1"/>
-      <c r="BH10" s="1"/>
-      <c r="BI10" s="1"/>
+      <c r="BE10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BF10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BG10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BH10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI10" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -2754,13 +2868,13 @@
         <v>37</v>
       </c>
       <c r="AZ11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BA11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BA11" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="BB11" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="BC11" s="1" t="s">
         <v>37</v>
@@ -2768,11 +2882,21 @@
       <c r="BD11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BE11" s="1"/>
-      <c r="BF11" s="1"/>
-      <c r="BG11" s="1"/>
-      <c r="BH11" s="1"/>
-      <c r="BI11" s="1"/>
+      <c r="BE11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BF11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BG11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BH11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI11" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -2929,13 +3053,13 @@
         <v>37</v>
       </c>
       <c r="AZ12" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="BB12" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="BC12" s="1" t="s">
         <v>37</v>
@@ -2943,11 +3067,21 @@
       <c r="BD12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BE12" s="1"/>
-      <c r="BF12" s="1"/>
-      <c r="BG12" s="1"/>
-      <c r="BH12" s="1"/>
-      <c r="BI12" s="1"/>
+      <c r="BE12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI12" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -3113,16 +3247,26 @@
         <v>57</v>
       </c>
       <c r="BC13" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="BD13" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="BE13" s="1"/>
-      <c r="BF13" s="1"/>
-      <c r="BG13" s="1"/>
-      <c r="BH13" s="1"/>
-      <c r="BI13" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="BE13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="BI13" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -3293,11 +3437,21 @@
       <c r="BD14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BE14" s="1"/>
-      <c r="BF14" s="1"/>
-      <c r="BG14" s="1"/>
-      <c r="BH14" s="1"/>
-      <c r="BI14" s="1"/>
+      <c r="BE14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="BH14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BI14" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -3454,25 +3608,38 @@
         <v>37</v>
       </c>
       <c r="AZ15" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BA15" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BB15" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BC15" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BD15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE15" s="1"/>
-      <c r="BF15" s="1"/>
-      <c r="BG15" s="1"/>
-      <c r="BH15" s="1"/>
-      <c r="BI15" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="BE15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BG15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BI15" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="63:63" x14ac:dyDescent="0.35">
+      <c r="BK20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="51">

</xml_diff>